<commit_message>
Added all of Brian Bunting to Unknown collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/UNKNOWN COLLECTION.xlsx
+++ b/Photographic Archive/UNKNOWN COLLECTION.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>identifier</t>
   </si>
@@ -52,13 +52,58 @@
   </si>
   <si>
     <t>COLLECTIONS</t>
+  </si>
+  <si>
+    <t>316A-HP</t>
+  </si>
+  <si>
+    <t>S-9B | 3.25</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPH</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Correspondence to Brian Bunting from other persons PHOTOGRAPH</t>
+  </si>
+  <si>
+    <t>MCH07-136-2-34</t>
+  </si>
+  <si>
+    <t>315A-HP</t>
+  </si>
+  <si>
+    <t>Funeral and Memorial Services/Moses Kotane PHOTOGRAPH</t>
+  </si>
+  <si>
+    <t>MCH07-131-5-68</t>
+  </si>
+  <si>
+    <t>314A-HP</t>
+  </si>
+  <si>
+    <t>MCH07-131-5-67</t>
+  </si>
+  <si>
+    <t>313A-HP</t>
+  </si>
+  <si>
+    <t>MCH07-131-5-66</t>
+  </si>
+  <si>
+    <t>312A-HP</t>
+  </si>
+  <si>
+    <t>MCH07-131-5-65</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +123,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -93,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,14 +152,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,6 +542,156 @@
         <v>11</v>
       </c>
       <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>